<commit_message>
fix bug RnD in 2015
</commit_message>
<xml_diff>
--- a/data/99. analyzes/excel/all_pharma_summarize.xlsx
+++ b/data/99. analyzes/excel/all_pharma_summarize.xlsx
@@ -722,10 +722,10 @@
         <v>70963.85000000001</v>
       </c>
       <c r="H3" t="n">
-        <v>6834851.539999999</v>
+        <v>5809991.16</v>
       </c>
       <c r="I3" t="n">
-        <v>9749358.629999999</v>
+        <v>8724498.25</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -751,10 +751,10 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>229351.8599999999</v>
+        <v>143574.7499999999</v>
       </c>
       <c r="I4" t="n">
-        <v>988589.3199999999</v>
+        <v>902812.21</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -878,28 +878,28 @@
         <v>18</v>
       </c>
       <c r="B9" t="n">
-        <v>2333324.59</v>
+        <v>2637611.63</v>
       </c>
       <c r="C9" t="n">
-        <v>7214682.939999999</v>
+        <v>7854002.02</v>
       </c>
       <c r="D9" t="n">
-        <v>155296.57</v>
+        <v>160848.95</v>
       </c>
       <c r="E9" t="n">
-        <v>197450.7499999999</v>
+        <v>208207.6499999999</v>
       </c>
       <c r="F9" t="n">
-        <v>1057913.93</v>
+        <v>1318222.22</v>
       </c>
       <c r="G9" t="n">
-        <v>39629.67</v>
+        <v>42723.4</v>
       </c>
       <c r="H9" t="n">
-        <v>10060783</v>
+        <v>13683143.1</v>
       </c>
       <c r="I9" t="n">
-        <v>21059081.45</v>
+        <v>25904758.97</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1087,22 +1087,22 @@
         <v>4225756.82</v>
       </c>
       <c r="D16" t="n">
-        <v>88050.64000000001</v>
+        <v>71151.64000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>498123.25</v>
+        <v>456841.25</v>
       </c>
       <c r="F16" t="n">
-        <v>1257749.82</v>
+        <v>1211741.82</v>
       </c>
       <c r="G16" t="n">
-        <v>55476.04000000001</v>
+        <v>53692.04000000001</v>
       </c>
       <c r="H16" t="n">
         <v>2866582.130000001</v>
       </c>
       <c r="I16" t="n">
-        <v>12414064.98</v>
+        <v>12308091.98</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1145,22 +1145,22 @@
         <v>671635.22</v>
       </c>
       <c r="D18" t="n">
-        <v>685999.6800000004</v>
+        <v>702898.6800000004</v>
       </c>
       <c r="E18" t="n">
-        <v>528572.1700000003</v>
+        <v>569854.1700000003</v>
       </c>
       <c r="F18" t="n">
-        <v>466586.64</v>
+        <v>512594.64</v>
       </c>
       <c r="G18" t="n">
-        <v>17509.39000000001</v>
+        <v>19293.39000000001</v>
       </c>
       <c r="H18" t="n">
         <v>2016003.189999998</v>
       </c>
       <c r="I18" t="n">
-        <v>5007835.499999999</v>
+        <v>5113808.499999999</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1418,10 +1418,10 @@
         <v>41641.53</v>
       </c>
       <c r="H27" t="n">
-        <v>5069507.579999999</v>
+        <v>3265417.13</v>
       </c>
       <c r="I27" t="n">
-        <v>12302506.35</v>
+        <v>10498415.9</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1516,28 +1516,28 @@
         <v>40</v>
       </c>
       <c r="B31" t="n">
-        <v>6202069</v>
+        <v>6593064</v>
       </c>
       <c r="C31" t="n">
-        <v>2541347</v>
+        <v>2702347</v>
       </c>
       <c r="D31" t="n">
-        <v>47805</v>
+        <v>56516</v>
       </c>
       <c r="E31" t="n">
-        <v>114360</v>
+        <v>132514</v>
       </c>
       <c r="F31" t="n">
-        <v>598751</v>
+        <v>701953</v>
       </c>
       <c r="G31" t="n">
-        <v>30627</v>
+        <v>51796</v>
       </c>
       <c r="H31" t="n">
-        <v>2125147</v>
+        <v>4364712</v>
       </c>
       <c r="I31" t="n">
-        <v>11660106</v>
+        <v>14602902</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1632,19 +1632,19 @@
         <v>44</v>
       </c>
       <c r="B35" t="n">
-        <v>530352.3</v>
+        <v>538729.3</v>
       </c>
       <c r="C35" t="n">
-        <v>3095443.8</v>
+        <v>3542678.8</v>
       </c>
       <c r="D35" t="n">
         <v>201759.4000000002</v>
       </c>
       <c r="E35" t="n">
-        <v>426843.9599999996</v>
+        <v>427367.9599999996</v>
       </c>
       <c r="F35" t="n">
-        <v>311141.5</v>
+        <v>313493.5</v>
       </c>
       <c r="G35" t="n">
         <v>610.7</v>
@@ -1653,7 +1653,7 @@
         <v>-1.862645149230957e-09</v>
       </c>
       <c r="I35" t="n">
-        <v>4566151.659999999</v>
+        <v>5024639.659999999</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1737,10 +1737,10 @@
         <v>133556.44</v>
       </c>
       <c r="H38" t="n">
-        <v>10993479.45</v>
+        <v>6709520.630000005</v>
       </c>
       <c r="I38" t="n">
-        <v>24745889.48</v>
+        <v>20461930.66</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1882,10 +1882,10 @@
         <v>295664.7299999999</v>
       </c>
       <c r="H43" t="n">
-        <v>45963126.17</v>
+        <v>36429450.62</v>
       </c>
       <c r="I43" t="n">
-        <v>78272281.55000001</v>
+        <v>68738606.00000001</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2041,25 +2041,25 @@
         <v>3018048.12</v>
       </c>
       <c r="C49" t="n">
-        <v>7422215.749999999</v>
+        <v>7435532.749999999</v>
       </c>
       <c r="D49" t="n">
-        <v>1771085.39</v>
+        <v>1817230.39</v>
       </c>
       <c r="E49" t="n">
-        <v>597663.9300000002</v>
+        <v>628350.9300000002</v>
       </c>
       <c r="F49" t="n">
-        <v>2271604.96</v>
+        <v>4010453.96</v>
       </c>
       <c r="G49" t="n">
-        <v>174551.23</v>
+        <v>235359.23</v>
       </c>
       <c r="H49" t="n">
-        <v>16692534.28</v>
+        <v>23690643.28</v>
       </c>
       <c r="I49" t="n">
-        <v>31947703.66</v>
+        <v>40835618.66</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2085,10 +2085,10 @@
         <v>35393.96</v>
       </c>
       <c r="H50" t="n">
-        <v>683348.0799999996</v>
+        <v>19548.86999999965</v>
       </c>
       <c r="I50" t="n">
-        <v>3180153.5</v>
+        <v>2516354.29</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2317,10 +2317,10 @@
         <v>9997.339999999998</v>
       </c>
       <c r="H58" t="n">
-        <v>2864638.47</v>
+        <v>1790540.42</v>
       </c>
       <c r="I58" t="n">
-        <v>6149574.76</v>
+        <v>5075476.71</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2592,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>6834851.54</v>
+        <v>5809991.16</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>229351.86</v>
+        <v>143574.75</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3018,25 +3018,25 @@
         <v>71</v>
       </c>
       <c r="C23" t="n">
-        <v>2333324.59</v>
+        <v>2637611.63</v>
       </c>
       <c r="D23" t="n">
-        <v>7214682.939999999</v>
+        <v>7854002.02</v>
       </c>
       <c r="E23" t="n">
-        <v>104776.46</v>
+        <v>109200.46</v>
       </c>
       <c r="F23" t="n">
-        <v>14016.83</v>
+        <v>14520.03</v>
       </c>
       <c r="G23" t="n">
-        <v>343143.3</v>
+        <v>454925.15</v>
       </c>
       <c r="H23" t="n">
-        <v>9794.060000000001</v>
+        <v>10267.86</v>
       </c>
       <c r="I23" t="n">
-        <v>10019738.18</v>
+        <v>11080527.15</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3051,19 +3051,19 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>50520.11000000001</v>
+        <v>51648.49000000001</v>
       </c>
       <c r="F24" t="n">
-        <v>183433.92</v>
+        <v>193687.62</v>
       </c>
       <c r="G24" t="n">
-        <v>714770.63</v>
+        <v>863297.0700000001</v>
       </c>
       <c r="H24" t="n">
-        <v>29835.61</v>
+        <v>32455.54</v>
       </c>
       <c r="I24" t="n">
-        <v>978560.2700000001</v>
+        <v>1141088.72</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3090,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>10060783</v>
+        <v>13683143.1</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3632,19 +3632,19 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>84763.01000000001</v>
+        <v>67864.01000000001</v>
       </c>
       <c r="F45" t="n">
-        <v>446408.66</v>
+        <v>405126.66</v>
       </c>
       <c r="G45" t="n">
-        <v>924662.7999999998</v>
+        <v>878654.7999999998</v>
       </c>
       <c r="H45" t="n">
-        <v>53501.63</v>
+        <v>51717.63</v>
       </c>
       <c r="I45" t="n">
-        <v>1509336.1</v>
+        <v>1403363.1</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3798,19 +3798,19 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>259962.5000000003</v>
+        <v>276861.5000000003</v>
       </c>
       <c r="F51" t="n">
-        <v>432544.6300000002</v>
+        <v>473826.6300000002</v>
       </c>
       <c r="G51" t="n">
-        <v>349406.89</v>
+        <v>395414.89</v>
       </c>
       <c r="H51" t="n">
-        <v>16759.44</v>
+        <v>18543.44</v>
       </c>
       <c r="I51" t="n">
-        <v>1058673.46</v>
+        <v>1164646.46</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -4557,7 +4557,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="n">
-        <v>5069507.58</v>
+        <v>3265417.13</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -4817,10 +4817,10 @@
         <v>71</v>
       </c>
       <c r="C88" t="n">
-        <v>6202069</v>
+        <v>6593064</v>
       </c>
       <c r="D88" t="n">
-        <v>2541347</v>
+        <v>2702347</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -4829,13 +4829,13 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>349009</v>
+        <v>349997</v>
       </c>
       <c r="H88" t="n">
         <v>29</v>
       </c>
       <c r="I88" t="n">
-        <v>9092454</v>
+        <v>9645437</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4850,19 +4850,19 @@
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>47805</v>
+        <v>56516</v>
       </c>
       <c r="F89" t="n">
-        <v>114360</v>
+        <v>132514</v>
       </c>
       <c r="G89" t="n">
-        <v>249742</v>
+        <v>351956</v>
       </c>
       <c r="H89" t="n">
-        <v>30598</v>
+        <v>51767</v>
       </c>
       <c r="I89" t="n">
-        <v>442505</v>
+        <v>592753</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="n">
-        <v>2125147</v>
+        <v>4364712</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -5149,10 +5149,10 @@
         <v>71</v>
       </c>
       <c r="C100" t="n">
-        <v>530352.3</v>
+        <v>538729.3</v>
       </c>
       <c r="D100" t="n">
-        <v>3055143.8</v>
+        <v>3502378.8</v>
       </c>
       <c r="E100" t="n">
         <v>4147.6</v>
@@ -5167,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="n">
-        <v>3635821</v>
+        <v>4091433</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -5185,16 +5185,16 @@
         <v>197611.8000000002</v>
       </c>
       <c r="F101" t="n">
-        <v>417177.6599999997</v>
+        <v>417701.6599999997</v>
       </c>
       <c r="G101" t="n">
-        <v>274630.5</v>
+        <v>276982.5</v>
       </c>
       <c r="H101" t="n">
         <v>610.7</v>
       </c>
       <c r="I101" t="n">
-        <v>930330.659999999</v>
+        <v>933206.659999999</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -5470,7 +5470,7 @@
         <v>0</v>
       </c>
       <c r="I111" t="n">
-        <v>10993479.45</v>
+        <v>6709520.63</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -5885,7 +5885,7 @@
         <v>0</v>
       </c>
       <c r="I126" t="n">
-        <v>45963126.17</v>
+        <v>36429450.62</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -6314,22 +6314,22 @@
         <v>3018048.12</v>
       </c>
       <c r="D142" t="n">
-        <v>7422215.749999999</v>
+        <v>7435532.749999999</v>
       </c>
       <c r="E142" t="n">
-        <v>1585779.22</v>
+        <v>1588413.22</v>
       </c>
       <c r="F142" t="n">
         <v>246133.16</v>
       </c>
       <c r="G142" t="n">
-        <v>1454036.66</v>
+        <v>1457836.66</v>
       </c>
       <c r="H142" t="n">
-        <v>56936.35000000001</v>
+        <v>57061.35000000001</v>
       </c>
       <c r="I142" t="n">
-        <v>13783149.26</v>
+        <v>13803025.26</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -6344,19 +6344,19 @@
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>185306.1699999999</v>
+        <v>228817.1699999999</v>
       </c>
       <c r="F143" t="n">
-        <v>351530.77</v>
+        <v>382217.77</v>
       </c>
       <c r="G143" t="n">
-        <v>817568.3</v>
+        <v>2552617.3</v>
       </c>
       <c r="H143" t="n">
-        <v>117614.88</v>
+        <v>178297.88</v>
       </c>
       <c r="I143" t="n">
-        <v>1472020.119999999</v>
+        <v>3341950.119999999</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -6383,7 +6383,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="n">
-        <v>16692534.28</v>
+        <v>23690643.28</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -6466,7 +6466,7 @@
         <v>0</v>
       </c>
       <c r="I147" t="n">
-        <v>683348.0800000001</v>
+        <v>19548.87</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -7130,7 +7130,7 @@
         <v>0</v>
       </c>
       <c r="I171" t="n">
-        <v>2864638.47</v>
+        <v>1790540.42</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -7679,7 +7679,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>6834851.54</v>
+        <v>5809991.16</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -7816,7 +7816,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>229351.86</v>
+        <v>143574.75</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -8375,25 +8375,25 @@
         <v>71</v>
       </c>
       <c r="C37" t="n">
-        <v>2322126.59</v>
+        <v>2626413.63</v>
       </c>
       <c r="D37" t="n">
-        <v>7138593.939999999</v>
+        <v>7777913.02</v>
       </c>
       <c r="E37" t="n">
-        <v>104659.46</v>
+        <v>109083.46</v>
       </c>
       <c r="F37" t="n">
-        <v>14016.83</v>
+        <v>14520.03</v>
       </c>
       <c r="G37" t="n">
-        <v>343084.3</v>
+        <v>454866.15</v>
       </c>
       <c r="H37" t="n">
-        <v>8048.06</v>
+        <v>8521.860000000001</v>
       </c>
       <c r="I37" t="n">
-        <v>9930529.18</v>
+        <v>10991318.15</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -8435,19 +8435,19 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>43533.11000000001</v>
+        <v>44661.49000000001</v>
       </c>
       <c r="F39" t="n">
-        <v>142544.92</v>
+        <v>152798.62</v>
       </c>
       <c r="G39" t="n">
-        <v>638121.63</v>
+        <v>786648.0700000001</v>
       </c>
       <c r="H39" t="n">
-        <v>27349.61</v>
+        <v>29969.54</v>
       </c>
       <c r="I39" t="n">
-        <v>851549.2700000001</v>
+        <v>1014077.72</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -8501,7 +8501,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>10060783</v>
+        <v>13683143.1</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -9340,19 +9340,19 @@
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>84763.01000000001</v>
+        <v>67864.01000000001</v>
       </c>
       <c r="F72" t="n">
-        <v>367402.0100000001</v>
+        <v>326120.0100000001</v>
       </c>
       <c r="G72" t="n">
-        <v>786225.5599999999</v>
+        <v>740217.5599999999</v>
       </c>
       <c r="H72" t="n">
-        <v>43054.51</v>
+        <v>41270.51</v>
       </c>
       <c r="I72" t="n">
-        <v>1281445.09</v>
+        <v>1175472.09</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -9614,19 +9614,19 @@
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>250974.2900000004</v>
+        <v>267873.2900000004</v>
       </c>
       <c r="F82" t="n">
-        <v>432457.5100000002</v>
+        <v>473739.5100000002</v>
       </c>
       <c r="G82" t="n">
-        <v>326952.41</v>
+        <v>372960.41</v>
       </c>
       <c r="H82" t="n">
-        <v>15307.48</v>
+        <v>17091.48</v>
       </c>
       <c r="I82" t="n">
-        <v>1025691.69</v>
+        <v>1131664.69</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -10832,7 +10832,7 @@
         <v>0</v>
       </c>
       <c r="I126" t="n">
-        <v>5069507.58</v>
+        <v>3265417.13</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -11254,10 +11254,10 @@
         <v>71</v>
       </c>
       <c r="C142" t="n">
-        <v>5724807</v>
+        <v>6115802</v>
       </c>
       <c r="D142" t="n">
-        <v>2378901</v>
+        <v>2539901</v>
       </c>
       <c r="E142" t="n">
         <v>0</v>
@@ -11266,13 +11266,13 @@
         <v>0</v>
       </c>
       <c r="G142" t="n">
-        <v>273612</v>
+        <v>274600</v>
       </c>
       <c r="H142" t="n">
         <v>29</v>
       </c>
       <c r="I142" t="n">
-        <v>8377349</v>
+        <v>8930332</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -11314,19 +11314,19 @@
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>39256</v>
+        <v>47967</v>
       </c>
       <c r="F144" t="n">
-        <v>89160</v>
+        <v>107314</v>
       </c>
       <c r="G144" t="n">
-        <v>234974</v>
+        <v>337188</v>
       </c>
       <c r="H144" t="n">
-        <v>26572</v>
+        <v>47741</v>
       </c>
       <c r="I144" t="n">
-        <v>389962</v>
+        <v>540210</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -11380,7 +11380,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="n">
-        <v>2125147</v>
+        <v>4364712</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -11802,10 +11802,10 @@
         <v>71</v>
       </c>
       <c r="C162" t="n">
-        <v>427170</v>
+        <v>435547</v>
       </c>
       <c r="D162" t="n">
-        <v>3055143.8</v>
+        <v>3502378.8</v>
       </c>
       <c r="E162" t="n">
         <v>4147.6</v>
@@ -11820,7 +11820,7 @@
         <v>0</v>
       </c>
       <c r="I162" t="n">
-        <v>3532638.7</v>
+        <v>3988250.7</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -11865,16 +11865,16 @@
         <v>197611.8000000002</v>
       </c>
       <c r="F164" t="n">
-        <v>386464.4999999997</v>
+        <v>386988.4999999997</v>
       </c>
       <c r="G164" t="n">
-        <v>271408.5</v>
+        <v>273760.5</v>
       </c>
       <c r="H164" t="n">
         <v>610.7</v>
       </c>
       <c r="I164" t="n">
-        <v>895795.499999999</v>
+        <v>898671.499999999</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -12339,7 +12339,7 @@
         <v>0</v>
       </c>
       <c r="I181" t="n">
-        <v>10993479.45</v>
+        <v>6709520.63</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -12970,7 +12970,7 @@
         <v>0</v>
       </c>
       <c r="I204" t="n">
-        <v>45963126.17</v>
+        <v>36429450.62</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -13669,22 +13669,22 @@
         <v>2962540.51</v>
       </c>
       <c r="D230" t="n">
-        <v>7420752.799999999</v>
+        <v>7434069.799999999</v>
       </c>
       <c r="E230" t="n">
-        <v>1585371.79</v>
+        <v>1588005.79</v>
       </c>
       <c r="F230" t="n">
         <v>241319.01</v>
       </c>
       <c r="G230" t="n">
-        <v>1448786.66</v>
+        <v>1452586.66</v>
       </c>
       <c r="H230" t="n">
-        <v>56936.35000000001</v>
+        <v>57061.35000000001</v>
       </c>
       <c r="I230" t="n">
-        <v>13715707.12</v>
+        <v>13735583.12</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -13726,19 +13726,19 @@
         <v>0</v>
       </c>
       <c r="E232" t="n">
-        <v>173851.7799999999</v>
+        <v>217362.7799999999</v>
       </c>
       <c r="F232" t="n">
-        <v>329942.25</v>
+        <v>360629.25</v>
       </c>
       <c r="G232" t="n">
-        <v>752861.3</v>
+        <v>2487910.3</v>
       </c>
       <c r="H232" t="n">
-        <v>114606.71</v>
+        <v>175289.71</v>
       </c>
       <c r="I232" t="n">
-        <v>1371262.039999999</v>
+        <v>3241192.039999999</v>
       </c>
     </row>
     <row r="233" spans="1:9">
@@ -13792,7 +13792,7 @@
         <v>0</v>
       </c>
       <c r="I234" t="n">
-        <v>16692534.28</v>
+        <v>23690643.28</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -13929,7 +13929,7 @@
         <v>0</v>
       </c>
       <c r="I239" t="n">
-        <v>683348.0800000001</v>
+        <v>19548.87</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -14971,7 +14971,7 @@
         <v>0</v>
       </c>
       <c r="I277" t="n">
-        <v>2864638.47</v>
+        <v>1790540.42</v>
       </c>
     </row>
     <row r="278" spans="1:9">
@@ -15570,22 +15570,22 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>5853074.320000002</v>
+        <v>1792837.71</v>
       </c>
       <c r="C13" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" t="n">
-        <v>3694408.53</v>
+        <v>1121669.38</v>
       </c>
       <c r="E13" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="n">
-        <v>9547482.850000001</v>
+        <v>2914507.09</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -15610,22 +15610,22 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B15" t="n">
-        <v>1792837.71</v>
+        <v>5853074.320000002</v>
       </c>
       <c r="C15" t="n">
         <v>62</v>
       </c>
       <c r="D15" t="n">
-        <v>1121669.38</v>
+        <v>3588435.53</v>
       </c>
       <c r="E15" t="n">
         <v>38</v>
       </c>
       <c r="F15" t="n">
-        <v>2914507.09</v>
+        <v>9441509.850000001</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -15710,202 +15710,202 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>4007512.7</v>
+        <v>9074098.449999999</v>
       </c>
       <c r="C20" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" t="n">
-        <v>1314133</v>
+        <v>3147517.42</v>
       </c>
       <c r="E20" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F20" t="n">
-        <v>5321645.7</v>
+        <v>12221615.87</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B21" t="n">
-        <v>5476783.77</v>
+        <v>4007512.7</v>
       </c>
       <c r="C21" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" t="n">
-        <v>1756215</v>
+        <v>1314133</v>
       </c>
       <c r="E21" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F21" t="n">
-        <v>7232998.77</v>
+        <v>5321645.7</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B22" t="n">
-        <v>4111109.15</v>
+        <v>5476783.77</v>
       </c>
       <c r="C22" t="n">
         <v>76</v>
       </c>
       <c r="D22" t="n">
-        <v>1288259.33</v>
+        <v>1756215</v>
       </c>
       <c r="E22" t="n">
         <v>24</v>
       </c>
       <c r="F22" t="n">
-        <v>5399368.48</v>
+        <v>7232998.77</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B23" t="n">
-        <v>1115787</v>
+        <v>7823038</v>
       </c>
       <c r="C23" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" t="n">
-        <v>333749</v>
+        <v>2415152</v>
       </c>
       <c r="E23" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F23" t="n">
-        <v>1449536</v>
+        <v>10238190</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B24" t="n">
-        <v>1946085.003</v>
+        <v>4111109.15</v>
       </c>
       <c r="C24" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D24" t="n">
-        <v>519837</v>
+        <v>1288259.33</v>
       </c>
       <c r="E24" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F24" t="n">
-        <v>2465922.003</v>
+        <v>5399368.48</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B25" t="n">
-        <v>7823038</v>
+        <v>1115787</v>
       </c>
       <c r="C25" t="n">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25" t="n">
-        <v>1711921</v>
+        <v>333749</v>
       </c>
       <c r="E25" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F25" t="n">
-        <v>9534959</v>
+        <v>1449536</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B26" t="n">
-        <v>700781.8</v>
+        <v>1946085.003</v>
       </c>
       <c r="C26" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D26" t="n">
-        <v>141124.46</v>
+        <v>519837</v>
       </c>
       <c r="E26" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F26" t="n">
-        <v>841906.26</v>
+        <v>2465922.003</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4113940.199999999</v>
+      </c>
+      <c r="C27" t="n">
+        <v>82</v>
+      </c>
+      <c r="D27" t="n">
+        <v>910699.46</v>
+      </c>
+      <c r="E27" t="n">
         <v>18</v>
       </c>
-      <c r="B27" t="n">
-        <v>9074098.449999999</v>
-      </c>
-      <c r="C27" t="n">
-        <v>83</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1924200</v>
-      </c>
-      <c r="E27" t="n">
-        <v>17</v>
-      </c>
       <c r="F27" t="n">
-        <v>10998298.45</v>
+        <v>5024639.659999999</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B28" t="n">
-        <v>5574450</v>
+        <v>700781.8</v>
       </c>
       <c r="C28" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" t="n">
-        <v>899597</v>
+        <v>141124.46</v>
       </c>
       <c r="E28" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F28" t="n">
-        <v>6474047</v>
+        <v>841906.26</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B29" t="n">
-        <v>777442.9199999999</v>
+        <v>1043682.4</v>
       </c>
       <c r="C29" t="n">
         <v>86</v>
       </c>
       <c r="D29" t="n">
-        <v>127490.45</v>
+        <v>164740.92</v>
       </c>
       <c r="E29" t="n">
         <v>14</v>
       </c>
       <c r="F29" t="n">
-        <v>904933.3699999999</v>
+        <v>1208423.32</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -15930,222 +15930,222 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B31" t="n">
-        <v>1043682.4</v>
+        <v>777442.9199999999</v>
       </c>
       <c r="C31" t="n">
         <v>86</v>
       </c>
       <c r="D31" t="n">
-        <v>164740.92</v>
+        <v>127490.45</v>
       </c>
       <c r="E31" t="n">
         <v>14</v>
       </c>
       <c r="F31" t="n">
-        <v>1208423.32</v>
+        <v>904933.3699999999</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2125655</v>
+        <v>5574450</v>
       </c>
       <c r="C32" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32" t="n">
-        <v>296046</v>
+        <v>899597</v>
       </c>
       <c r="E32" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F32" t="n">
-        <v>2421701</v>
+        <v>6474047</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B33" t="n">
-        <v>1183172.64</v>
+        <v>15086880.16</v>
       </c>
       <c r="C33" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D33" t="n">
-        <v>143245.89</v>
+        <v>2058095.22</v>
       </c>
       <c r="E33" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F33" t="n">
-        <v>1326418.53</v>
+        <v>17144975.38</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B34" t="n">
-        <v>4113940.199999999</v>
+        <v>2125655</v>
       </c>
       <c r="C34" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" t="n">
-        <v>452211.46</v>
+        <v>296046</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F34" t="n">
-        <v>4566151.659999999</v>
+        <v>2421701</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="B35" t="n">
-        <v>4364000.770000003</v>
+        <v>1183172.64</v>
       </c>
       <c r="C35" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" t="n">
-        <v>444776.85</v>
+        <v>143245.89</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F35" t="n">
-        <v>4808777.620000003</v>
+        <v>1326418.53</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B36" t="n">
-        <v>393396.49</v>
+        <v>9808754.42</v>
       </c>
       <c r="C36" t="n">
         <v>91</v>
       </c>
       <c r="D36" t="n">
-        <v>39023.2</v>
+        <v>949686.63</v>
       </c>
       <c r="E36" t="n">
         <v>9</v>
       </c>
       <c r="F36" t="n">
-        <v>432419.69</v>
+        <v>10758441.05</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B37" t="n">
-        <v>573285.3199999998</v>
+        <v>393396.49</v>
       </c>
       <c r="C37" t="n">
         <v>91</v>
       </c>
       <c r="D37" t="n">
-        <v>54880.67</v>
+        <v>39023.2</v>
       </c>
       <c r="E37" t="n">
         <v>9</v>
       </c>
       <c r="F37" t="n">
-        <v>628165.9899999999</v>
+        <v>432419.69</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B38" t="n">
-        <v>9808754.42</v>
+        <v>4364000.770000003</v>
       </c>
       <c r="C38" t="n">
         <v>91</v>
       </c>
       <c r="D38" t="n">
-        <v>949686.63</v>
+        <v>444776.85</v>
       </c>
       <c r="E38" t="n">
         <v>9</v>
       </c>
       <c r="F38" t="n">
-        <v>10758441.05</v>
+        <v>4808777.620000003</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B39" t="n">
-        <v>2106295.33</v>
+        <v>573285.3199999998</v>
       </c>
       <c r="C39" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D39" t="n">
-        <v>172926.435</v>
+        <v>54880.67</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
-        <v>2279221.765</v>
+        <v>628165.9899999999</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B40" t="n">
-        <v>3709689.9</v>
+        <v>2106295.33</v>
       </c>
       <c r="C40" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" t="n">
-        <v>284678</v>
+        <v>172926.435</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F40" t="n">
-        <v>3994367.9</v>
+        <v>2279221.765</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B41" t="n">
-        <v>958584.46</v>
+        <v>3709689.9</v>
       </c>
       <c r="C41" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D41" t="n">
-        <v>59769.24</v>
+        <v>284678</v>
       </c>
       <c r="E41" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>1018353.7</v>
+        <v>3994367.9</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -16170,62 +16170,62 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B43" t="n">
-        <v>709498.2400000001</v>
+        <v>958584.46</v>
       </c>
       <c r="C43" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43" t="n">
-        <v>36711.34</v>
+        <v>59769.24</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
-        <v>746209.5800000001</v>
+        <v>1018353.7</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B44" t="n">
-        <v>17356429.99999999</v>
+        <v>2921429.489999999</v>
       </c>
       <c r="C44" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D44" t="n">
-        <v>686504.55</v>
+        <v>176375.82</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
-        <v>18042934.54999999</v>
+        <v>3097805.309999999</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B45" t="n">
-        <v>3168810.92</v>
+        <v>709498.2400000001</v>
       </c>
       <c r="C45" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45" t="n">
-        <v>116125.37</v>
+        <v>36711.34</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
-        <v>3284936.29</v>
+        <v>746209.5800000001</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -16250,62 +16250,62 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B47" t="n">
-        <v>921002.2</v>
+        <v>3168810.92</v>
       </c>
       <c r="C47" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D47" t="n">
-        <v>27134</v>
+        <v>116125.37</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F47" t="n">
-        <v>948136.2</v>
+        <v>3284936.29</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>2921429.489999999</v>
+        <v>17356429.99999999</v>
       </c>
       <c r="C48" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" t="n">
-        <v>70402.82000000001</v>
+        <v>686504.55</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F48" t="n">
-        <v>2991832.309999999</v>
+        <v>18042934.54999999</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B49" t="n">
-        <v>15086880.16</v>
+        <v>921002.2</v>
       </c>
       <c r="C49" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D49" t="n">
-        <v>168289.22</v>
+        <v>27134</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
-        <v>15255169.38</v>
+        <v>948136.2</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -16410,42 +16410,42 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B55" t="n">
-        <v>12080548.41</v>
+        <v>344076</v>
       </c>
       <c r="C55" t="n">
         <v>100</v>
       </c>
       <c r="D55" t="n">
-        <v>484.79</v>
+        <v>1576</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>12081033.2</v>
+        <v>345652</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B56" t="n">
-        <v>344076</v>
+        <v>12080548.41</v>
       </c>
       <c r="C56" t="n">
         <v>100</v>
       </c>
       <c r="D56" t="n">
-        <v>1576</v>
+        <v>484.79</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>345652</v>
+        <v>12081033.2</v>
       </c>
     </row>
     <row r="57" spans="1:6">

</xml_diff>